<commit_message>
update ahang ond doku
</commit_message>
<xml_diff>
--- a/40_Arbeitjournal/Arbeitsjournal.xlsx
+++ b/40_Arbeitjournal/Arbeitsjournal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b7schal\Documents\GitHub\GEM\40_Arbeitjournal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\GitHub\GEM\40_Arbeitjournal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826BFB5-E5A8-4400-B057-85E091483736}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -257,7 +258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,9 +381,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -393,6 +391,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -674,11 +675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +730,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
@@ -747,7 +748,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
@@ -765,7 +766,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -785,7 +786,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -803,7 +804,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
@@ -821,7 +822,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -841,7 +842,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -859,7 +860,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -877,7 +878,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -897,7 +898,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
@@ -915,7 +916,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
@@ -933,7 +934,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -953,7 +954,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
@@ -971,7 +972,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -989,7 +990,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1009,7 +1010,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1027,7 +1028,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +1046,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1065,7 +1066,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1083,7 +1084,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="3" t="s">
         <v>49</v>
       </c>
@@ -1101,7 +1102,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1121,7 +1122,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
@@ -1139,7 +1140,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
@@ -1157,7 +1158,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1177,7 +1178,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1195,7 +1196,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -1215,7 +1216,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
@@ -1233,7 +1234,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="3" t="s">
         <v>55</v>
       </c>
@@ -1251,7 +1252,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -1267,7 +1268,7 @@
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="2" t="s">
         <v>24</v>
       </c>
@@ -1285,7 +1286,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="3" t="s">
         <v>51</v>
       </c>
@@ -1323,7 +1324,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="3" t="s">
         <v>56</v>
       </c>
@@ -1361,7 +1362,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="2" t="s">
         <v>71</v>
       </c>
@@ -1379,7 +1380,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="3" t="s">
         <v>67</v>
       </c>
@@ -1397,7 +1398,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1417,7 +1418,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="2" t="s">
         <v>75</v>
       </c>
@@ -1435,7 +1436,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="3" t="s">
         <v>72</v>
       </c>
@@ -1473,7 +1474,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="2" t="s">
         <v>57</v>
       </c>
@@ -1491,7 +1492,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="3" t="s">
         <v>58</v>
       </c>
@@ -1569,7 +1570,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="2" t="s">
         <v>66</v>
       </c>
@@ -1587,7 +1588,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="3" t="s">
         <v>67</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>7</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>42</v>
@@ -1625,7 +1626,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="2" t="s">
         <v>70</v>
       </c>
@@ -1643,15 +1644,15 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
+      <c r="A52" s="17"/>
       <c r="B52" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>42</v>
@@ -1694,11 +1695,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A2:A4"/>
@@ -1706,6 +1702,11 @@
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A41"/>

</xml_diff>